<commit_message>
Cleaning out archived proxy outputs - Superceded outputs moved to Dropbox archive
</commit_message>
<xml_diff>
--- a/Archive_OPGEEProxyCH4Version/AF Analysis/AF Analysis (Autosaved).xlsx
+++ b/Archive_OPGEEProxyCH4Version/AF Analysis/AF Analysis (Autosaved).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruthe\Dropbox\Doctoral\Projects\Research Projects\OPGEE\0_OPGEE_Matlab\Version 3\AF Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruthe\BU_methane_model\Archive_OPGEEProxyCH4Version\AF Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43306E82-17E4-4EAA-BC97-C3B5A5BC7444}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19596" windowHeight="10116" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$11:$V$11</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -230,8 +230,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +244,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -334,26 +340,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,27 +640,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -698,7 +704,7 @@
         <v>0.43586590247037216</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -742,13 +748,13 @@
         <v>0.28978834048409668</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>7</v>
       </c>
@@ -801,7 +807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -861,7 +867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>210</v>
       </c>
@@ -924,7 +930,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>420</v>
       </c>
@@ -987,7 +993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>575</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>535</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>160</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>345</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>430</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>220</v>
       </c>
@@ -1365,7 +1371,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>360</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>540</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>745</v>
       </c>
@@ -1554,7 +1560,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>395</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>515</v>
       </c>
@@ -1680,19 +1686,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1707,7 +1713,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>40</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>41</v>
       </c>
@@ -1777,7 +1783,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <v>0</v>
       </c>
@@ -1817,7 +1823,7 @@
         <v>0.35157711761084487</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>0</v>
       </c>
@@ -1857,7 +1863,7 @@
         <v>1.6010504679636397</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>0</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>2.1189388205044</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
         <v>0</v>
       </c>
@@ -1937,7 +1943,7 @@
         <v>3.3481572839445453</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <v>0</v>
       </c>
@@ -1977,7 +1983,7 @@
         <v>0.52160510539520311</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>0</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>0.88926529748041494</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2029,7 +2035,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>43</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>40</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>41</v>
       </c>
@@ -2134,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2147,7 +2153,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>43</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>40</v>
       </c>
@@ -2227,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>41</v>
       </c>
@@ -2272,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2284,7 +2290,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2299,7 +2305,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>40</v>
       </c>
@@ -2334,7 +2340,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>41</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2381,7 +2387,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D49" s="1">
         <f t="shared" ref="D49:D55" si="4">IF($V18="OIL",(D18/D$7),(D18/D$6))</f>
         <v>0.70908339471967408</v>
@@ -2419,7 +2425,7 @@
         <v>0.79353339839018699</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D50" s="1">
         <f t="shared" si="4"/>
         <v>1.1990791402556107</v>
@@ -2457,7 +2463,7 @@
         <v>3.0664493701059676</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D51" s="1">
         <f t="shared" si="4"/>
         <v>1.6905527565810692</v>
@@ -2495,7 +2501,7 @@
         <v>2.481022682173097</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D52" s="1">
         <f t="shared" si="4"/>
         <v>0.89133405823848055</v>
@@ -2533,7 +2539,7 @@
         <v>3.4925850903026365</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D53" s="1">
         <f t="shared" si="4"/>
         <v>0.40717495959659417</v>
@@ -2571,7 +2577,7 @@
         <v>1.2224046397047212E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D54" s="1">
         <f t="shared" si="4"/>
         <v>1.6751159993125966</v>
@@ -2609,7 +2615,7 @@
         <v>2.1819172669834295</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D55" s="1">
         <f t="shared" si="4"/>
         <v>0.66815144766146994</v>
@@ -2647,7 +2653,7 @@
         <v>1.1396697365516963</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -2659,7 +2665,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>40</v>
       </c>
@@ -2729,7 +2735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>41</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -2777,7 +2783,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>43</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="8" t="s">
         <v>40</v>
       </c>
@@ -2857,7 +2863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>41</v>
       </c>
@@ -2902,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -2914,7 +2920,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -2926,7 +2932,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -2938,7 +2944,7 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -2950,7 +2956,7 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -2962,7 +2968,7 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -2975,7 +2981,7 @@
       <c r="M69" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:V11">
+  <autoFilter ref="A11:V11" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A12:V24">
       <sortCondition ref="V11"/>
     </sortState>
@@ -3125,46 +3131,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="14" t="s">
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="15">
@@ -3180,8 +3186,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="15">
@@ -3197,8 +3203,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="15">
@@ -3214,8 +3220,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="15">
@@ -3231,8 +3237,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="15">
@@ -3248,8 +3254,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="15">
@@ -3265,8 +3271,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="15">
@@ -3282,8 +3288,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="15">
@@ -3299,20 +3305,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>4</v>
       </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
         <v>4</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>0</v>
       </c>
     </row>
@@ -3326,16 +3332,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3380,7 +3386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3470,7 +3476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>

</xml_diff>